<commit_message>
Production test on new run
</commit_message>
<xml_diff>
--- a/Chips2016-01.xlsx
+++ b/Chips2016-01.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="155">
   <si>
     <t>Final status</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>power suply</t>
+  </si>
+  <si>
+    <t>FLEX DAMIC</t>
   </si>
 </sst>
 </file>
@@ -935,8 +938,8 @@
   <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4210,6 +4213,9 @@
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>113</v>
+      </c>
+      <c r="B206" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="C206" t="s">
         <v>147</v>

</xml_diff>